<commit_message>
Revisão Tang 13: revisão de títulos
Tornar os títulos mais claros para representar o que representa
Trocar “primitivo” por “inicial”
</commit_message>
<xml_diff>
--- a/Files/Texto/cores.xlsx
+++ b/Files/Texto/cores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\INF01131-Monografia\Files\Texto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79B62D1-91C4-40C5-9C43-BBDCAB2B2568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A76C872-B087-432E-8B13-AF7BAB4B380B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>#E0E0E0</t>
   </si>
   <si>
-    <t>#CCFF33</t>
-  </si>
-  <si>
-    <t>#8B0000</t>
-  </si>
-  <si>
     <t>#D66615</t>
   </si>
   <si>
@@ -50,9 +44,6 @@
   </si>
   <si>
     <t>#3EC200</t>
-  </si>
-  <si>
-    <t>#000000</t>
   </si>
   <si>
     <t>#0055FF</t>
@@ -233,22 +224,19 @@
     <t>Não Computação</t>
   </si>
   <si>
-    <t>Sem Paridade</t>
-  </si>
-  <si>
-    <t>Eletiva optativa</t>
-  </si>
-  <si>
-    <t>Eletiva livre</t>
-  </si>
-  <si>
-    <t>Sem categoria</t>
-  </si>
-  <si>
     <t>Categoria</t>
   </si>
   <si>
     <t>Correto</t>
+  </si>
+  <si>
+    <t>Eletiva Livre</t>
+  </si>
+  <si>
+    <t>Sem Categoria</t>
+  </si>
+  <si>
+    <t>Eletiva Optativa</t>
   </si>
 </sst>
 </file>
@@ -272,13 +260,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -286,8 +267,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="56">
+  <fills count="57">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,18 +289,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCFF33"/>
-        <bgColor rgb="FFCCFF33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8B0000"/>
-        <bgColor rgb="FF8B0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD66615"/>
         <bgColor rgb="FFD66615"/>
       </patternFill>
@@ -355,9 +330,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid"/>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0055FF"/>
         <bgColor rgb="FF0055FF"/>
@@ -613,6 +585,30 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFE3580E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFC72508"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF8B0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFCCFF33"/>
       </patternFill>
     </fill>
   </fills>
@@ -786,100 +782,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="53" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="54" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -888,6 +808,79 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="42" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="45" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="46" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="48" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="50" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="53" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="54" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="54" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="55" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,7 +1198,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -1236,265 +1229,255 @@
     </row>
     <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="66" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
+      <c r="B2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="68" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="63" t="s">
+      <c r="G2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="65"/>
+      <c r="H2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="72" t="s">
-        <v>23</v>
+      <c r="B3" s="15"/>
+      <c r="C3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="70" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="I3" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="72" t="s">
-        <v>66</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="73">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>7</v>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="I4" s="71"/>
+      <c r="J4" s="70"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="73">
-        <v>1</v>
-      </c>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="22" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="50" t="s">
         <v>4</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="73">
-        <v>2</v>
-      </c>
-      <c r="C6" s="29" t="s">
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="25" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="62" t="s">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>11</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="73">
-        <v>3</v>
-      </c>
-      <c r="C7" s="32" t="s">
+      <c r="B7" s="9">
+        <v>4</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="28" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>14</v>
+        <v>56</v>
+      </c>
+      <c r="H7" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="58" t="s">
+        <v>15</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="73">
-        <v>4</v>
-      </c>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="9">
+        <v>5</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="31" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>18</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="67"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="73">
-        <v>5</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="B9" s="9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="34" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>6</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="68"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="B10" s="73">
-        <v>6</v>
-      </c>
-      <c r="C10" s="41" t="s">
+      <c r="B10" s="9">
+        <v>7</v>
+      </c>
+      <c r="C10" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="37" t="s">
         <v>41</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>6</v>
-      </c>
+      <c r="G10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="69"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="73">
-        <v>7</v>
-      </c>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="9">
+        <v>8</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="40" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="1"/>
@@ -1506,74 +1489,66 @@
     </row>
     <row r="12" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="73">
-        <v>8</v>
-      </c>
-      <c r="C12" s="47" t="s">
+      <c r="B12" s="9">
+        <v>9</v>
+      </c>
+      <c r="C12" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="43" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="61" t="s">
-        <v>56</v>
+      <c r="G12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="73">
-        <v>9</v>
-      </c>
-      <c r="C13" s="50" t="s">
+      <c r="B13" s="10">
+        <v>10</v>
+      </c>
+      <c r="C13" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="46" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="56" t="s">
-        <v>3</v>
+      <c r="G13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="63" t="s">
+        <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="74">
-        <v>10</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>53</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="57" t="s">
-        <v>7</v>
+      <c r="G14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="64" t="s">
+        <v>8</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1586,48 +1561,43 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="73" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="58" t="s">
-        <v>11</v>
+      <c r="G15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="65" t="s">
+        <v>12</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="73" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="59" t="s">
-        <v>15</v>
+      <c r="G16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="66" t="s">
+        <v>16</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="74" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="60" t="s">
-        <v>19</v>
-      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Revisão Tang 14: remover cor errada de conflito
Remover a cor “#000” do conflito de Demanda colocar a mesma cor que o conflito de sala
</commit_message>
<xml_diff>
--- a/Files/Texto/cores.xlsx
+++ b/Files/Texto/cores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\INF01131-Monografia\Files\Texto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A76C872-B087-432E-8B13-AF7BAB4B380B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86E432-7FEF-42C1-AAEB-152607BA182D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -807,24 +807,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -881,6 +863,24 @@
     <xf numFmtId="0" fontId="3" fillId="54" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="55" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -1229,28 +1229,28 @@
     </row>
     <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="6" t="s">
         <v>52</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="15"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="6" t="s">
         <v>60</v>
       </c>
@@ -1278,24 +1278,24 @@
       <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="70"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="64"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1303,26 +1303,26 @@
       <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="16" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="49" t="s">
+      <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="44" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="1"/>
@@ -1332,26 +1332,26 @@
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="H6" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="55" t="s">
+      <c r="J6" s="49" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="1"/>
@@ -1361,26 +1361,26 @@
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="22" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="58" t="s">
+      <c r="J7" s="52" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="1"/>
@@ -1390,26 +1390,26 @@
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="25" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="56" t="s">
+      <c r="H8" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="67"/>
+      <c r="J8" s="61"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1417,26 +1417,26 @@
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="28" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="68"/>
+      <c r="J9" s="62"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1444,26 +1444,26 @@
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="31" t="s">
         <v>41</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="61" t="s">
+      <c r="H10" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="62" t="s">
+      <c r="I10" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="69"/>
+      <c r="J10" s="63"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1471,13 +1471,13 @@
       <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="34" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="1"/>
@@ -1492,13 +1492,13 @@
       <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="37" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="1"/>
@@ -1517,20 +1517,20 @@
       <c r="B13" s="10">
         <v>10</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="46" t="s">
+      <c r="E13" s="40" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="63" t="s">
+      <c r="H13" s="57" t="s">
         <v>1</v>
       </c>
       <c r="I13" s="1"/>
@@ -1547,7 +1547,7 @@
       <c r="G14" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="64" t="s">
+      <c r="H14" s="58" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="1"/>
@@ -1564,7 +1564,7 @@
       <c r="G15" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="65" t="s">
+      <c r="H15" s="59" t="s">
         <v>12</v>
       </c>
       <c r="I15" s="1"/>
@@ -1581,7 +1581,7 @@
       <c r="G16" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="66" t="s">
+      <c r="H16" s="60" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="1"/>
@@ -1600,7 +1600,7 @@
       <c r="I17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>

</xml_diff>